<commit_message>
added June 21 and other archive files related to task 1 and task 2
</commit_message>
<xml_diff>
--- a/Work History.xlsx
+++ b/Work History.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3AAF29-AEBE-4E01-8C0E-5E42EAD289B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1FDDDC-98D0-4F1A-97BC-ED1DF6E95FDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Overview" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -40,10 +41,43 @@
     <t>OTBI report - Master details and Action Links-practice task for  task2</t>
   </si>
   <si>
-    <t>Customer detail Analysis with OTBI report - Master details and Action Links-task2</t>
-  </si>
-  <si>
-    <t>task1 has to be completed within today</t>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>MORNING TASK</t>
+  </si>
+  <si>
+    <t>AFTERNOON TASK</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>COMMENTS</t>
+  </si>
+  <si>
+    <t>Bi report multiple layouts</t>
+  </si>
+  <si>
+    <t>Documentation for both</t>
+  </si>
+  <si>
+    <t>details and action links)</t>
+  </si>
+  <si>
+    <t>task1(BI reports) and task2 (otbi -master</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -76,12 +110,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -89,11 +123,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -101,14 +181,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -384,32 +507,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="2" customWidth="1"/>
     <col min="2" max="2" width="71.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="98.7109375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="55.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44363</v>
       </c>
@@ -419,28 +546,97 @@
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44364</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>44365</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83FCC79-1ACF-4D2D-A945-7B1EAD946E60}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>44368</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
created June 24 folder, added excel task1 documenta
</commit_message>
<xml_diff>
--- a/Work History.xlsx
+++ b/Work History.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1FDDDC-98D0-4F1A-97BC-ED1DF6E95FDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394EBC33-CBC8-490E-BAAE-ED2AE97C2A6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Overview" sheetId="2" r:id="rId2"/>
+    <sheet name="Over-view" sheetId="2" r:id="rId2"/>
+    <sheet name="Task Summary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -78,6 +79,83 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Task Question</t>
+  </si>
+  <si>
+    <t>Task 1 for multiple latyouts for all customer/suppliers for  a module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(such as receivable,purchasing,PO,AP invoice module etc,. ). Using only a </t>
+  </si>
+  <si>
+    <t>parameter as BUSINESS_UNIT.Using Bi Publisher</t>
+  </si>
+  <si>
+    <t>details for all BU's(hardcoded).Each page has a detail of Customer/Supplier detail</t>
+  </si>
+  <si>
+    <t>TASK1</t>
+  </si>
+  <si>
+    <t>TASK2</t>
+  </si>
+  <si>
+    <t>TASK3</t>
+  </si>
+  <si>
+    <t>TASK4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each page has a detail of Customer/Supplier detail such as their details like </t>
+  </si>
+  <si>
+    <t>name, address, city,country, postalcode followed by this, a table should</t>
+  </si>
+  <si>
+    <t>Using task1 datamodel: create a single sheet template for all customer/supplier</t>
+  </si>
+  <si>
+    <t>Create a multilayout EXCEL Report for the same datamodel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for task1 and then click EXCEL preview in BI Publisher menu in MS Word. 2)  Here we don't need to </t>
+  </si>
+  <si>
+    <t>create any template,simply use rtf template for task1 and then excel preview will generate output)</t>
+  </si>
+  <si>
+    <t>consist of some meaningfull columns and data.(HINT: 1)use the rtf template loaded with data model)</t>
+  </si>
+  <si>
+    <t>Table analysis</t>
+  </si>
+  <si>
+    <t>Multiple Layout analysis and Task1 completed</t>
+  </si>
+  <si>
+    <t>Excel task1</t>
+  </si>
+  <si>
+    <t>Excel task2</t>
+  </si>
+  <si>
+    <t>Documentation for 1. multiple layout in rtf template
+2. bursting scenarios
+3. master details in otbi
+4. action links in otbi
+5. excel template report
+6. Multiple sheet excel output with rtf template</t>
+  </si>
+  <si>
+    <t>TASK Number</t>
+  </si>
+  <si>
+    <t>Task Date</t>
+  </si>
+  <si>
+    <t>Bursting has to be done within today</t>
   </si>
 </sst>
 </file>
@@ -101,7 +179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,6 +189,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -173,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -195,32 +279,21 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -507,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +635,62 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>44367</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44370</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44371</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -575,7 +703,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +740,7 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
@@ -623,19 +751,146 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="11" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="11" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C4">
-    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3FE8EE-F31D-4416-8EB0-9A448F0250C7}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="93.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>44370</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>44371</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
created 26 June folder added TASK 6 files to 26 June folder
</commit_message>
<xml_diff>
--- a/Work History.xlsx
+++ b/Work History.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394EBC33-CBC8-490E-BAAE-ED2AE97C2A6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CE0CDE-34DE-4798-AEFF-F989BBEA7ACE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,17 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Tasks completed</t>
-  </si>
-  <si>
-    <t>Tasks remaining</t>
-  </si>
-  <si>
     <t>Bi report for receivables module-task1</t>
   </si>
   <si>
@@ -141,7 +135,29 @@
     <t>Excel task2</t>
   </si>
   <si>
-    <t>Documentation for 1. multiple layout in rtf template
+    <t>TASK Number</t>
+  </si>
+  <si>
+    <t>Task Date</t>
+  </si>
+  <si>
+    <t>Bursting has to be done within today</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Tasks remaining @ eod</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Documentation for:
+1. multiple layout in rtf template
 2. bursting scenarios
 3. master details in otbi
 4. action links in otbi
@@ -149,20 +165,96 @@
 6. Multiple sheet excel output with rtf template</t>
   </si>
   <si>
-    <t>TASK Number</t>
-  </si>
-  <si>
-    <t>Task Date</t>
-  </si>
-  <si>
-    <t>Bursting has to be done within today</t>
+    <t>KAVINNARESH.RENGARAJ@CHAINSYS.COM</t>
+  </si>
+  <si>
+    <t>HTTPS://WWW.GITHUB.COM/KAVINKAVIN16/FUSION</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KAVIN NARESH G R </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2595</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TRAINEE CONSULTANT ORACLE TECHNICAL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TRAINER 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: ARUN </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TRAINER 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: MOHAMMEDASIFKHANA</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +270,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,8 +319,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -253,11 +380,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -274,9 +439,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -289,23 +451,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCC99"/>
+      <color rgb="FFFCF7CE"/>
+      <color rgb="FFFAD0E5"/>
+      <color rgb="FFD5D3F7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -580,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,109 +770,148 @@
     <col min="2" max="2" width="71.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="55.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="16.85546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>44363</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>44364</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>44367</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>44368</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44370</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>44369</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>44370</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>44371</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B17" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
+      <c r="D17" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{2BE2EFD6-D895-4AD6-9D18-65574FCFA397}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{49F825E2-FDF0-44B5-869C-73AD85F20521}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -703,7 +920,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,46 +935,46 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>44368</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>44368</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -768,10 +985,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3FE8EE-F31D-4416-8EB0-9A448F0250C7}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,14 +999,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>40</v>
+      <c r="A1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -801,10 +1018,10 @@
         <v>44363</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -812,82 +1029,80 @@
         <v>44364</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44368</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>44370</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>44370</v>
-      </c>
-      <c r="B11" s="13" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>44371</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>44371</v>
-      </c>
-      <c r="B17" s="13" t="s">
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created 28 June folder , added TASK6 catalog file
</commit_message>
<xml_diff>
--- a/Work History.xlsx
+++ b/Work History.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CE0CDE-34DE-4798-AEFF-F989BBEA7ACE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CA6F4A-4D50-411C-86D6-E099FBD3B7C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -248,6 +248,15 @@
       </rPr>
       <t>: MOHAMMEDASIFKHANA</t>
     </r>
+  </si>
+  <si>
+    <t>Reports on multiple dependency parameters (not less than 5 params)</t>
+  </si>
+  <si>
+    <t>Bursting completed and results mail came</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -758,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,6 +912,20 @@
       </c>
       <c r="D17" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44373</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added task 6 catalog and report template files to 28 June folder
</commit_message>
<xml_diff>
--- a/Work History.xlsx
+++ b/Work History.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CA6F4A-4D50-411C-86D6-E099FBD3B7C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5725C666-79DE-4135-ABBD-970A919047E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -257,6 +257,18 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>output came somehow</t>
+  </si>
+  <si>
+    <t>TASK J5</t>
+  </si>
+  <si>
+    <t>BURSTING</t>
+  </si>
+  <si>
+    <t>TASK6</t>
   </si>
 </sst>
 </file>
@@ -431,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -450,7 +462,6 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -477,6 +488,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -767,9 +790,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -786,27 +809,27 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>49</v>
       </c>
     </row>
@@ -824,10 +847,10 @@
       <c r="D9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -904,7 +927,7 @@
       <c r="A17" s="1">
         <v>44371</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -926,6 +949,17 @@
       </c>
       <c r="D18" s="2" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1008,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3FE8EE-F31D-4416-8EB0-9A448F0250C7}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,111 +1056,229 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="22" t="s">
         <v>37</v>
       </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
+      <c r="C4" s="20"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="19">
         <v>44363</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="19">
         <v>44364</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="20" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="19">
         <v>44368</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="C7" s="20"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
+      <c r="C8" s="20"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="C9" s="20"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="C10" s="20"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="21">
         <v>44370</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="11" t="s">
         <v>21</v>
       </c>
+      <c r="C12" s="20"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="C13" s="20"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="C14" s="20"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="C15" s="20"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="21">
         <v>44371</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
       <c r="B17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+      <c r="C17" s="20"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="C18" s="20"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
+      <c r="C19" s="20"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="20"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
       <c r="B21" t="s">
         <v>31</v>
       </c>
+      <c r="C21" s="20"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="C22" s="20"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
+        <v>44371</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="C24" s="20"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
+        <v>44372</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="20"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="20"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="20"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="20"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="20"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="20"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="20"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="20"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="20"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="20"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="20"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="20"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="20"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="20"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="20"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>